<commit_message>
Artikel: Berkas Pajak: eBupot PPh Unifikasi: Pengaturan
</commit_message>
<xml_diff>
--- a/assets/posts/pajak/2022/06/Teliti-2022-SSE.xlsx
+++ b/assets/posts/pajak/2022/06/Teliti-2022-SSE.xlsx
@@ -11,7 +11,7 @@
     <sheet name="SSE" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">SSE!$A$1:$G$21</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">SSE!$A$1:$G$24</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t xml:space="preserve">Surat Setoran Elektronik</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t xml:space="preserve">Tanggal Potong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gabungan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Setor Masa</t>
   </si>
   <si>
     <t xml:space="preserve">Tanggal Setor</t>
@@ -293,7 +299,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -382,7 +388,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -390,14 +396,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -410,12 +408,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -495,10 +497,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="2:3"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -659,47 +661,72 @@
       <c r="F16" s="16"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B17" s="21"/>
-      <c r="C17" s="10" t="s">
+      <c r="B17" s="25"/>
+      <c r="C17" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="25" t="n">
+      <c r="D17" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="27" t="n">
         <v>44706</v>
       </c>
-      <c r="F17" s="23"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B18" s="13"/>
-      <c r="C18" s="14" t="s">
+      <c r="F17" s="28"/>
+    </row>
+    <row r="18" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B19" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="26" t="s">
+      <c r="C19" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="16"/>
-      <c r="G18" s="18"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B19" s="27"/>
-      <c r="C19" s="28" t="s">
+      <c r="D19" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="11" t="n">
+        <v>6738210</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B21" s="13"/>
+      <c r="C21" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="F19" s="30"/>
-    </row>
-    <row r="20" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
-    <row r="21" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
+      <c r="D21" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="16"/>
+      <c r="G21" s="18"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B22" s="25"/>
+      <c r="C22" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F22" s="28"/>
+    </row>
+    <row r="23" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
+    <row r="24" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="B2:C2"/>

</xml_diff>

<commit_message>
Artikel: Berkas Pajak: Pengisian eBupot PPh Unifikasi
</commit_message>
<xml_diff>
--- a/assets/posts/pajak/2022/06/Teliti-2022-SSE.xlsx
+++ b/assets/posts/pajak/2022/06/Teliti-2022-SSE.xlsx
@@ -11,7 +11,7 @@
     <sheet name="SSE" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">SSE!$A$1:$G$24</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">SSE!$A$1:$G$22</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,10 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
-  <si>
-    <t xml:space="preserve">Surat Setoran Elektronik</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
   <si>
     <t xml:space="preserve">Current: 2022</t>
   </si>
@@ -112,7 +109,7 @@
     <numFmt numFmtId="168" formatCode="0\:"/>
     <numFmt numFmtId="169" formatCode="dd\ mmm\ yyyy&quot;, &quot;ddd"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -133,13 +130,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="11"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -169,18 +159,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB3B"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -299,7 +283,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -308,59 +292,55 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -368,7 +348,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,19 +356,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -396,19 +376,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -416,7 +396,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -436,7 +416,7 @@
       <rgbColor rgb="FFFF0000"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFEB3B"/>
+      <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -497,10 +477,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="pageBreakPreview" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="2:3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -514,224 +494,217 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+    <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2"/>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4" t="s">
+      <c r="C2" s="3"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
+      <c r="C6" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="10" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="B7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="15"/>
+    </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B8" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="10" t="s">
+      <c r="B8" s="12"/>
+      <c r="C8" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="14" t="n">
+        <v>411128</v>
+      </c>
+      <c r="F8" s="15"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="14" t="n">
+        <v>403</v>
+      </c>
+      <c r="F9" s="15"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="15"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B11" s="12"/>
+      <c r="C11" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E11" s="16" t="n">
+        <v>100000</v>
+      </c>
+      <c r="F11" s="15"/>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="B12" s="12"/>
+      <c r="C12" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B13" s="20"/>
+      <c r="C13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="22"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B14" s="12"/>
+      <c r="C14" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="15"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B15" s="24"/>
+      <c r="C15" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E15" s="26" t="n">
+        <v>44706</v>
+      </c>
+      <c r="F15" s="27"/>
+    </row>
+    <row r="16" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17" s="10" t="n">
+        <v>1000000</v>
+      </c>
+      <c r="F17" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="11" t="n">
-        <v>1000000</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B9" s="13"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="16"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B10" s="13"/>
-      <c r="C10" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="15" t="n">
-        <v>411128</v>
-      </c>
-      <c r="F10" s="16"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B11" s="13"/>
-      <c r="C11" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="15" t="n">
-        <v>403</v>
-      </c>
-      <c r="F11" s="16"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B12" s="13"/>
-      <c r="C12" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" s="16"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B13" s="13"/>
-      <c r="C13" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="17" t="n">
-        <v>100000</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="18"/>
-    </row>
-    <row r="14" customFormat="false" ht="22.7" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B14" s="13"/>
-      <c r="C14" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="20"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B15" s="21"/>
-      <c r="C15" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="23"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B16" s="13"/>
-      <c r="C16" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="16"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B17" s="25"/>
-      <c r="C17" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="27" t="n">
-        <v>44706</v>
-      </c>
-      <c r="F17" s="28"/>
-    </row>
-    <row r="18" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
+    </row>
+    <row r="18" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="B18" s="12"/>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="15"/>
+    </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B19" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" s="10" t="s">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="11" t="n">
-        <v>6738210</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B20" s="13"/>
-      <c r="C20" s="14"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="16"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B21" s="13"/>
-      <c r="C21" s="14" t="s">
+      <c r="D19" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="24" t="s">
+      <c r="F19" s="15"/>
+      <c r="G19" s="17"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+      <c r="B20" s="24"/>
+      <c r="C20" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="16"/>
-      <c r="G21" s="18"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B22" s="25"/>
-      <c r="C22" s="26" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="F22" s="28"/>
-    </row>
-    <row r="23" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
-    <row r="24" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
+      <c r="D20" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="27"/>
+    </row>
+    <row r="21" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
+    <row r="22" customFormat="false" ht="7.1" hidden="false" customHeight="true" outlineLevel="1" collapsed="false"/>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E12:F12"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>